<commit_message>
Creating spreadsheets for BUCS and balena code runs
</commit_message>
<xml_diff>
--- a/ParameterIndependent/InputSheetBalena.xlsx
+++ b/ParameterIndependent/InputSheetBalena.xlsx
@@ -12274,8 +12274,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12405,7 +12405,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>